<commit_message>
add context for section 5 of SDD
</commit_message>
<xml_diff>
--- a/Documentation/TimeSheets/week9/Huy Nguyen Week 9 Timesheet .xlsx
+++ b/Documentation/TimeSheets/week9/Huy Nguyen Week 9 Timesheet .xlsx
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="27">
   <si>
     <t>Hours Worked</t>
   </si>
@@ -95,6 +95,30 @@
   </si>
   <si>
     <t>4:00PM</t>
+  </si>
+  <si>
+    <t>12:00PM</t>
+  </si>
+  <si>
+    <t>Imporve and test robot before meeting</t>
+  </si>
+  <si>
+    <t>Research ant build file</t>
+  </si>
+  <si>
+    <t>5:00PM</t>
+  </si>
+  <si>
+    <t>Enhance follow track for automation mode</t>
+  </si>
+  <si>
+    <t>1:00PM</t>
+  </si>
+  <si>
+    <t>7:00PM</t>
+  </si>
+  <si>
+    <t>10:00PM</t>
   </si>
 </sst>
 </file>
@@ -707,7 +731,7 @@
   <dimension ref="B1:H19"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="B10" sqref="B10"/>
+      <selection activeCell="D13" sqref="D13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="19.95" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -769,15 +793,15 @@
       </c>
       <c r="C5" s="8">
         <f>SUBTOTAL(109,TimeSheet[Hours Worked])</f>
-        <v>2.5</v>
+        <v>12.5</v>
       </c>
       <c r="D5" s="8">
         <f>IFERROR(IF(C5&lt;=WorkweekHours,C5,WorkweekHours),"")</f>
-        <v>2.5</v>
+        <v>12</v>
       </c>
       <c r="E5" s="8">
         <f>IFERROR(C5-D5, "")</f>
-        <v>0</v>
+        <v>0.5</v>
       </c>
     </row>
     <row r="6" spans="2:8" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.3">
@@ -830,41 +854,71 @@
     </row>
     <row r="9" spans="2:8" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B9" s="10" t="s">
-        <v>16</v>
+        <v>20</v>
       </c>
       <c r="C9" s="13">
         <v>43011</v>
       </c>
       <c r="D9" s="11" t="s">
+        <v>19</v>
+      </c>
+      <c r="E9" s="11" t="s">
+        <v>15</v>
+      </c>
+      <c r="F9" s="12">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="10" spans="2:8" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B10" s="10" t="s">
+        <v>16</v>
+      </c>
+      <c r="C10" s="13">
+        <v>43011</v>
+      </c>
+      <c r="D10" s="11" t="s">
         <v>17</v>
       </c>
-      <c r="E9" s="11" t="s">
+      <c r="E10" s="11" t="s">
         <v>18</v>
       </c>
-      <c r="F9" s="12">
+      <c r="F10" s="12">
         <v>0.5</v>
       </c>
     </row>
-    <row r="10" spans="2:8" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B10" s="10"/>
-      <c r="C10" s="13"/>
-      <c r="D10" s="11"/>
-      <c r="E10" s="11"/>
-      <c r="F10" s="12"/>
-    </row>
     <row r="11" spans="2:8" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B11" s="10"/>
-      <c r="C11" s="13"/>
-      <c r="D11" s="11"/>
-      <c r="E11" s="11"/>
-      <c r="F11" s="12"/>
+      <c r="B11" s="10" t="s">
+        <v>21</v>
+      </c>
+      <c r="C11" s="13">
+        <v>43013</v>
+      </c>
+      <c r="D11" s="11" t="s">
+        <v>24</v>
+      </c>
+      <c r="E11" s="11" t="s">
+        <v>22</v>
+      </c>
+      <c r="F11" s="12">
+        <v>4</v>
+      </c>
     </row>
     <row r="12" spans="2:8" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B12" s="10"/>
-      <c r="C12" s="13"/>
-      <c r="D12" s="11"/>
-      <c r="E12" s="11"/>
-      <c r="F12" s="12"/>
+      <c r="B12" s="10" t="s">
+        <v>23</v>
+      </c>
+      <c r="C12" s="13">
+        <v>43015</v>
+      </c>
+      <c r="D12" s="11" t="s">
+        <v>25</v>
+      </c>
+      <c r="E12" s="11" t="s">
+        <v>26</v>
+      </c>
+      <c r="F12" s="12">
+        <v>3</v>
+      </c>
     </row>
     <row r="13" spans="2:8" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B13" s="10"/>
@@ -898,7 +952,7 @@
     </row>
   </sheetData>
   <dataValidations count="21">
-    <dataValidation allowBlank="1" showErrorMessage="1" sqref="C1:E1 D3:E3 F1:XFD5 A2:A1048576 G6:XFD1048576 B7:F14 B18:F1048576 B17:E17" xr:uid="{00000000-0002-0000-0000-000000000000}"/>
+    <dataValidation allowBlank="1" showErrorMessage="1" sqref="C1:E1 D3:E3 F1:XFD5 A2:A1048576 G6:XFD1048576 B17:E17 B18:F1048576 B7:F14" xr:uid="{00000000-0002-0000-0000-000000000000}"/>
     <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Enter Time Out in this column under this heading" sqref="E6" xr:uid="{00000000-0002-0000-0000-000001000000}"/>
     <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Hours Worked are automatically calculated in this column under this heading" sqref="F6" xr:uid="{00000000-0002-0000-0000-000002000000}"/>
     <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Enter Period Start Date in this cell" sqref="B3" xr:uid="{00000000-0002-0000-0000-000003000000}"/>

</xml_diff>